<commit_message>
Added some dummy data
Added some dummy data and formatted graph properly

also added approximate time i have been working on things so far (1 hr)
</commit_message>
<xml_diff>
--- a/Managment/Burndown.xlsx
+++ b/Managment/Burndown.xlsx
@@ -14,6 +14,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$H$2:$H$6</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$H$2:$H$6</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,24 +29,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Total Time</t>
   </si>
   <si>
-    <t>sprint 1</t>
+    <t>y</t>
   </si>
   <si>
-    <t>sprint 2</t>
+    <t>x</t>
   </si>
   <si>
-    <t>sprint 3</t>
+    <t>m</t>
   </si>
   <si>
-    <t>sprint 4</t>
+    <t>Sprint</t>
   </si>
   <si>
-    <t>sprint 5</t>
+    <t>after sprint</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Sprints until complete</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>Time Left</t>
   </si>
 </sst>
 </file>
@@ -111,6 +131,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Using some dummy data to create a rough burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -151,7 +200,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Work left</c:v>
+            <c:v>Hours per Sprint</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -164,46 +213,123 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:trendline>
+            <c:name>Current Work Rate</c:name>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="9"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="4"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.4785663024471105E-2"/>
+                  <c:y val="4.6066479452306221E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$15</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A117-49C8-B42B-AF8E205C2764}"/>
+              <c16:uniqueId val="{00000000-0A5F-458A-944A-22DEFCE4818A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Optimal Hours Per Sprint</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0A5F-458A-944A-22DEFCE4818A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -215,13 +341,77 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="449886984"/>
-        <c:axId val="449887968"/>
+        <c:gapWidth val="150"/>
+        <c:axId val="419120712"/>
+        <c:axId val="419121696"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Optimal Work Rate</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A5F-458A-944A-22DEFCE4818A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="419120712"/>
+        <c:axId val="419121696"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="449886984"/>
+        <c:axId val="419120712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -249,6 +439,10 @@
                 <a:r>
                   <a:rPr lang="en-AU"/>
                   <a:t>Sprint</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> number</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -318,15 +512,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449887968"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="419121696"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="449887968"/>
+        <c:axId val="419121696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,7 +560,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Hours</a:t>
+                  <a:t>Hours </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -432,8 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449886984"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="419120712"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -444,6 +636,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -522,7 +745,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -726,22 +949,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -911,6 +1135,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -979,19 +1214,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1028,20 +1264,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1356,60 +1592,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <f>24*7</f>
+        <v>168</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>H2-H3</f>
+        <v>42</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>B2</f>
+        <v>168</v>
+      </c>
+      <c r="I2">
+        <f>(G6-G2)/(I6-H2)</f>
+        <v>-2.3809523809523808E-2</v>
+      </c>
+      <c r="J2">
+        <f>1-(H2*I2)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <f>B2-E2</f>
+        <v>167</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <f>H3-H4</f>
+        <v>42</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f>(G3-J2)/I2</f>
+        <v>126</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <f>H4-H5</f>
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="0">(G4-$J$2)/$I$2</f>
+        <v>84</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5">
+        <f>H5-H6</f>
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="H6">
+        <f>(G6-$J$2)/$I$2</f>
         <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <f>(0-167.8)/-0.2</f>
+        <v>839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added matlab code to workout sprints left
now has projected sprints left
</commit_message>
<xml_diff>
--- a/Managment/Burndown.xlsx
+++ b/Managment/Burndown.xlsx
@@ -13,12 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$H$2:$H$6</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$H$2:$H$6</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Total Time</t>
   </si>
@@ -62,6 +58,9 @@
   </si>
   <si>
     <t>Time Left</t>
+  </si>
+  <si>
+    <t>Final sprint</t>
   </si>
 </sst>
 </file>
@@ -151,11 +150,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Using some dummy data to create a rough burndown</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> chart</a:t>
+              <a:t>Work Left</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -200,7 +195,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Hours per Sprint</c:v>
+            <c:v>Hours Left</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -212,58 +207,1026 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:name>Current Work Rate</c:name>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="9"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.4785663024471105E-2"/>
-                  <c:y val="4.6066479452306221E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$377</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="377"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$6</c:f>
@@ -276,60 +1239,18 @@
                 <c:pt idx="1">
                   <c:v>167</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0A5F-458A-944A-22DEFCE4818A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Optimal Hours Per Sprint</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$2:$H$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>168</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0A5F-458A-944A-22DEFCE4818A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -376,15 +1297,9 @@
                   <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>126</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -394,6 +1309,544 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0A5F-458A-944A-22DEFCE4818A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Projection</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="168"/>
+                <c:pt idx="0">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>166.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>164.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>162.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>159.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>158.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>157.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>156.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>155.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>154.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>153.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>152.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>151.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>150.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>149.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>148.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>147.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>146.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>145.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>144.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>143.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>142.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>141.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>140.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>139.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>138.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>137.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>136.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>135.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>134.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>133.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>132.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>131.5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>130.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>129.5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>128.5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>127.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>126.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>125.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>124.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>123.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>122.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>121.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>120.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>119.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>118.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>117.5</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>116.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>115.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>114.5</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>113.5</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>111.5</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>110.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>108.5</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>106.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>105.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>102.5</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>101.5</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>100.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>93.5</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>91.5</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>84.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-66A3-4BB4-A329-2AD9166664FB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -476,6 +1929,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -513,6 +1967,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="419121696"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -626,6 +2081,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="419120712"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1270,8 +2726,8 @@
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
@@ -1592,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +3103,7 @@
       </c>
       <c r="F2">
         <f>H2-H3</f>
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1657,12 +3113,12 @@
         <v>168</v>
       </c>
       <c r="I2">
-        <f>(G6-G2)/(I6-H2)</f>
-        <v>-2.3809523809523808E-2</v>
+        <f>(G4-G2)/(I6-H2)</f>
+        <v>-1.1904761904761904E-2</v>
       </c>
       <c r="J2">
         <f>1-(H2*I2)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1681,17 +3137,21 @@
       </c>
       <c r="F3">
         <f>H3-H4</f>
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
         <f>(G3-J2)/I2</f>
-        <v>126</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>B3-E3</f>
+        <v>167</v>
+      </c>
       <c r="D4">
         <v>3</v>
       </c>
@@ -1700,58 +3160,2749 @@
       </c>
       <c r="F4">
         <f>H4-H5</f>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H6" si="0">(G4-$J$2)/$I$2</f>
-        <v>84</v>
+        <f>(G4-$J$2)/$I$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <f>H5-H6</f>
-        <v>42</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <f>(G6-$J$2)/$I$2</f>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E7">
-        <f>(0-167.8)/-0.2</f>
-        <v>839</v>
+      <c r="E8">
+        <f>COUNT(Sheet2!A:A)</f>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B337"/>
+  <sheetViews>
+    <sheetView topLeftCell="A300" workbookViewId="0">
+      <selection sqref="A1:B337"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>167.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>166.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>165.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>164.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>163.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>162.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>159.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>158.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>156.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>155.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>154.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>153.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>151.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>150.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>149.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>147.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>146.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>144.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>143.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>141.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>140.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>139.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>138.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>134.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <v>133.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>132.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <v>131.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>129.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <v>128.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>126.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88">
+        <v>124.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90">
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92">
+        <v>122.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94">
+        <v>121.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96">
+        <v>120.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98">
+        <v>119.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>118.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102">
+        <v>117.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104">
+        <v>116.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106">
+        <v>115.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>108</v>
+      </c>
+      <c r="B108">
+        <v>114.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>109</v>
+      </c>
+      <c r="B109">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>112</v>
+      </c>
+      <c r="B112">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>113</v>
+      </c>
+      <c r="B113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>114</v>
+      </c>
+      <c r="B114">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>115</v>
+      </c>
+      <c r="B115">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>116</v>
+      </c>
+      <c r="B116">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>117</v>
+      </c>
+      <c r="B117">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>118</v>
+      </c>
+      <c r="B118">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>119</v>
+      </c>
+      <c r="B119">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>120</v>
+      </c>
+      <c r="B120">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>121</v>
+      </c>
+      <c r="B121">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>122</v>
+      </c>
+      <c r="B122">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>123</v>
+      </c>
+      <c r="B123">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>124</v>
+      </c>
+      <c r="B124">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>125</v>
+      </c>
+      <c r="B125">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>126</v>
+      </c>
+      <c r="B126">
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>127</v>
+      </c>
+      <c r="B127">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>128</v>
+      </c>
+      <c r="B128">
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>129</v>
+      </c>
+      <c r="B129">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>130</v>
+      </c>
+      <c r="B130">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>131</v>
+      </c>
+      <c r="B131">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>132</v>
+      </c>
+      <c r="B132">
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>133</v>
+      </c>
+      <c r="B133">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>134</v>
+      </c>
+      <c r="B134">
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>135</v>
+      </c>
+      <c r="B135">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>136</v>
+      </c>
+      <c r="B136">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>137</v>
+      </c>
+      <c r="B137">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144">
+        <v>96.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>150</v>
+      </c>
+      <c r="B150">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>151</v>
+      </c>
+      <c r="B151">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>152</v>
+      </c>
+      <c r="B152">
+        <v>92.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>153</v>
+      </c>
+      <c r="B153">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>154</v>
+      </c>
+      <c r="B154">
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>156</v>
+      </c>
+      <c r="B156">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>157</v>
+      </c>
+      <c r="B157">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>158</v>
+      </c>
+      <c r="B158">
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>159</v>
+      </c>
+      <c r="B159">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>160</v>
+      </c>
+      <c r="B160">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>161</v>
+      </c>
+      <c r="B161">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>162</v>
+      </c>
+      <c r="B162">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>163</v>
+      </c>
+      <c r="B163">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>164</v>
+      </c>
+      <c r="B164">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>165</v>
+      </c>
+      <c r="B165">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>166</v>
+      </c>
+      <c r="B166">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>167</v>
+      </c>
+      <c r="B167">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>168</v>
+      </c>
+      <c r="B168">
+        <v>84.5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>169</v>
+      </c>
+      <c r="B169">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>170</v>
+      </c>
+      <c r="B170">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>171</v>
+      </c>
+      <c r="B171">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>172</v>
+      </c>
+      <c r="B172">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>173</v>
+      </c>
+      <c r="B173">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>174</v>
+      </c>
+      <c r="B174">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>175</v>
+      </c>
+      <c r="B175">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>176</v>
+      </c>
+      <c r="B176">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>177</v>
+      </c>
+      <c r="B177">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>178</v>
+      </c>
+      <c r="B178">
+        <v>79.5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>179</v>
+      </c>
+      <c r="B179">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>180</v>
+      </c>
+      <c r="B180">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>181</v>
+      </c>
+      <c r="B181">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>182</v>
+      </c>
+      <c r="B182">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>183</v>
+      </c>
+      <c r="B183">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>184</v>
+      </c>
+      <c r="B184">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>185</v>
+      </c>
+      <c r="B185">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>186</v>
+      </c>
+      <c r="B186">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>187</v>
+      </c>
+      <c r="B187">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>188</v>
+      </c>
+      <c r="B188">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>189</v>
+      </c>
+      <c r="B189">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>190</v>
+      </c>
+      <c r="B190">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>191</v>
+      </c>
+      <c r="B191">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>192</v>
+      </c>
+      <c r="B192">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>193</v>
+      </c>
+      <c r="B193">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>194</v>
+      </c>
+      <c r="B194">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>195</v>
+      </c>
+      <c r="B195">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>196</v>
+      </c>
+      <c r="B196">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>197</v>
+      </c>
+      <c r="B197">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>198</v>
+      </c>
+      <c r="B198">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>199</v>
+      </c>
+      <c r="B199">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="B200">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>201</v>
+      </c>
+      <c r="B201">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>202</v>
+      </c>
+      <c r="B202">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>203</v>
+      </c>
+      <c r="B203">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>204</v>
+      </c>
+      <c r="B204">
+        <v>66.5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>205</v>
+      </c>
+      <c r="B205">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>206</v>
+      </c>
+      <c r="B206">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>207</v>
+      </c>
+      <c r="B207">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>208</v>
+      </c>
+      <c r="B208">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>209</v>
+      </c>
+      <c r="B209">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>210</v>
+      </c>
+      <c r="B210">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>211</v>
+      </c>
+      <c r="B211">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>212</v>
+      </c>
+      <c r="B212">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>213</v>
+      </c>
+      <c r="B213">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>214</v>
+      </c>
+      <c r="B214">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>215</v>
+      </c>
+      <c r="B215">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>216</v>
+      </c>
+      <c r="B216">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>217</v>
+      </c>
+      <c r="B217">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>218</v>
+      </c>
+      <c r="B218">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>219</v>
+      </c>
+      <c r="B219">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>220</v>
+      </c>
+      <c r="B220">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>221</v>
+      </c>
+      <c r="B221">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>222</v>
+      </c>
+      <c r="B222">
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>223</v>
+      </c>
+      <c r="B223">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>224</v>
+      </c>
+      <c r="B224">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>225</v>
+      </c>
+      <c r="B225">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>226</v>
+      </c>
+      <c r="B226">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>227</v>
+      </c>
+      <c r="B227">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>228</v>
+      </c>
+      <c r="B228">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>229</v>
+      </c>
+      <c r="B229">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>230</v>
+      </c>
+      <c r="B230">
+        <v>53.5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>231</v>
+      </c>
+      <c r="B231">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>232</v>
+      </c>
+      <c r="B232">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>233</v>
+      </c>
+      <c r="B233">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>234</v>
+      </c>
+      <c r="B234">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>235</v>
+      </c>
+      <c r="B235">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>236</v>
+      </c>
+      <c r="B236">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>237</v>
+      </c>
+      <c r="B237">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>238</v>
+      </c>
+      <c r="B238">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>239</v>
+      </c>
+      <c r="B239">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>240</v>
+      </c>
+      <c r="B240">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>241</v>
+      </c>
+      <c r="B241">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>242</v>
+      </c>
+      <c r="B242">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>243</v>
+      </c>
+      <c r="B243">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>244</v>
+      </c>
+      <c r="B244">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>245</v>
+      </c>
+      <c r="B245">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>246</v>
+      </c>
+      <c r="B246">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>247</v>
+      </c>
+      <c r="B247">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>248</v>
+      </c>
+      <c r="B248">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>249</v>
+      </c>
+      <c r="B249">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>250</v>
+      </c>
+      <c r="B250">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>251</v>
+      </c>
+      <c r="B251">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>252</v>
+      </c>
+      <c r="B252">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>253</v>
+      </c>
+      <c r="B253">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>254</v>
+      </c>
+      <c r="B254">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>255</v>
+      </c>
+      <c r="B255">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>256</v>
+      </c>
+      <c r="B256">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>257</v>
+      </c>
+      <c r="B257">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>258</v>
+      </c>
+      <c r="B258">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>259</v>
+      </c>
+      <c r="B259">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>260</v>
+      </c>
+      <c r="B260">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>261</v>
+      </c>
+      <c r="B261">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>262</v>
+      </c>
+      <c r="B262">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>263</v>
+      </c>
+      <c r="B263">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>264</v>
+      </c>
+      <c r="B264">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>265</v>
+      </c>
+      <c r="B265">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>266</v>
+      </c>
+      <c r="B266">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>267</v>
+      </c>
+      <c r="B267">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>268</v>
+      </c>
+      <c r="B268">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>269</v>
+      </c>
+      <c r="B269">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>270</v>
+      </c>
+      <c r="B270">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>271</v>
+      </c>
+      <c r="B271">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>272</v>
+      </c>
+      <c r="B272">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>273</v>
+      </c>
+      <c r="B273">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>274</v>
+      </c>
+      <c r="B274">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>275</v>
+      </c>
+      <c r="B275">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>276</v>
+      </c>
+      <c r="B276">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>277</v>
+      </c>
+      <c r="B277">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>278</v>
+      </c>
+      <c r="B278">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>279</v>
+      </c>
+      <c r="B279">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>280</v>
+      </c>
+      <c r="B280">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>281</v>
+      </c>
+      <c r="B281">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>282</v>
+      </c>
+      <c r="B282">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>283</v>
+      </c>
+      <c r="B283">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>284</v>
+      </c>
+      <c r="B284">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>285</v>
+      </c>
+      <c r="B285">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>286</v>
+      </c>
+      <c r="B286">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>287</v>
+      </c>
+      <c r="B287">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>288</v>
+      </c>
+      <c r="B288">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>289</v>
+      </c>
+      <c r="B289">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>290</v>
+      </c>
+      <c r="B290">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>291</v>
+      </c>
+      <c r="B291">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>292</v>
+      </c>
+      <c r="B292">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>293</v>
+      </c>
+      <c r="B293">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>294</v>
+      </c>
+      <c r="B294">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>295</v>
+      </c>
+      <c r="B295">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>296</v>
+      </c>
+      <c r="B296">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>297</v>
+      </c>
+      <c r="B297">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>298</v>
+      </c>
+      <c r="B298">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>299</v>
+      </c>
+      <c r="B299">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>300</v>
+      </c>
+      <c r="B300">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>301</v>
+      </c>
+      <c r="B301">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>302</v>
+      </c>
+      <c r="B302">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>303</v>
+      </c>
+      <c r="B303">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>304</v>
+      </c>
+      <c r="B304">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>305</v>
+      </c>
+      <c r="B305">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>306</v>
+      </c>
+      <c r="B306">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>307</v>
+      </c>
+      <c r="B307">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>308</v>
+      </c>
+      <c r="B308">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>309</v>
+      </c>
+      <c r="B309">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>310</v>
+      </c>
+      <c r="B310">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>311</v>
+      </c>
+      <c r="B311">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>312</v>
+      </c>
+      <c r="B312">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>313</v>
+      </c>
+      <c r="B313">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>314</v>
+      </c>
+      <c r="B314">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>315</v>
+      </c>
+      <c r="B315">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>316</v>
+      </c>
+      <c r="B316">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>317</v>
+      </c>
+      <c r="B317">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>318</v>
+      </c>
+      <c r="B318">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>319</v>
+      </c>
+      <c r="B319">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>320</v>
+      </c>
+      <c r="B320">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>321</v>
+      </c>
+      <c r="B321">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>322</v>
+      </c>
+      <c r="B322">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>323</v>
+      </c>
+      <c r="B323">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>324</v>
+      </c>
+      <c r="B324">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>325</v>
+      </c>
+      <c r="B325">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>326</v>
+      </c>
+      <c r="B326">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>327</v>
+      </c>
+      <c r="B327">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>328</v>
+      </c>
+      <c r="B328">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>329</v>
+      </c>
+      <c r="B329">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>330</v>
+      </c>
+      <c r="B330">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>331</v>
+      </c>
+      <c r="B331">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>332</v>
+      </c>
+      <c r="B332">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>333</v>
+      </c>
+      <c r="B333">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>334</v>
+      </c>
+      <c r="B334">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>335</v>
+      </c>
+      <c r="B335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>336</v>
+      </c>
+      <c r="B336">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>337</v>
+      </c>
+      <c r="B337">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to burndown chart data
main changes by Jon, misc fixes by Alex
</commit_message>
<xml_diff>
--- a/Managment/Burndown.xlsx
+++ b/Managment/Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\University\C workspace\EGB220-Robotracer\Managment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\workspace\EGB220-Robotracer\Managment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -102,7 +102,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -972,258 +993,6 @@
                 <c:pt idx="252">
                   <c:v>253</c:v>
                 </c:pt>
-                <c:pt idx="253">
-                  <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>255</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>257</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>258</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>259</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>261</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>263</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>268</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>269</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>271</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>272</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>274</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>277</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>278</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>281</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>282</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>285</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>286</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>287</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>289</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>291</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>292</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>293</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>294</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>295</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>296</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>297</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>298</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>299</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>302</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>304</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>307</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>309</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>311</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>312</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>313</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>314</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>315</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>319</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>321</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>323</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>324</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>326</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>327</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>328</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>329</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>331</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>332</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>333</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>335</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>336</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>337</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1237,13 +1006,13 @@
                   <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>167</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,9 +1066,12 @@
                   <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1332,513 +1104,768 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$1:$B$168</c:f>
+              <c:f>Sheet2!$B$1:$B$253</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="168"/>
+                <c:ptCount val="253"/>
                 <c:pt idx="0">
                   <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167.5</c:v>
+                  <c:v>167.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>167</c:v>
+                  <c:v>166.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>166.5</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>166</c:v>
+                  <c:v>165.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>165.5</c:v>
+                  <c:v>164.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>165</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>164.5</c:v>
+                  <c:v>163.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>164</c:v>
+                  <c:v>162.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>163.5</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>163</c:v>
+                  <c:v>161.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>162.5</c:v>
+                  <c:v>160.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>162</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>161.5</c:v>
+                  <c:v>159.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>161</c:v>
+                  <c:v>158.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160.5</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>157.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>159.5</c:v>
+                  <c:v>156.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>159</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>158.5</c:v>
+                  <c:v>155.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>158</c:v>
+                  <c:v>154.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>157.5</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>157</c:v>
+                  <c:v>153.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>156.5</c:v>
+                  <c:v>152.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>156</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>155.5</c:v>
+                  <c:v>151.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>155</c:v>
+                  <c:v>150.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>154.5</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>154</c:v>
+                  <c:v>149.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>153.5</c:v>
+                  <c:v>148.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>153</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>152.5</c:v>
+                  <c:v>147.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>152</c:v>
+                  <c:v>146.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>151.5</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>151</c:v>
+                  <c:v>145.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>150.5</c:v>
+                  <c:v>144.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>150</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>149.5</c:v>
+                  <c:v>143.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>149</c:v>
+                  <c:v>142.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>148.5</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>148</c:v>
+                  <c:v>141.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>147.5</c:v>
+                  <c:v>140.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>147</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>146.5</c:v>
+                  <c:v>139.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>146</c:v>
+                  <c:v>138.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>145.5</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>145</c:v>
+                  <c:v>137.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>144.5</c:v>
+                  <c:v>136.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>144</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>143.5</c:v>
+                  <c:v>135.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>143</c:v>
+                  <c:v>134.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>142.5</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>142</c:v>
+                  <c:v>133.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>141.5</c:v>
+                  <c:v>132.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>141</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>140.5</c:v>
+                  <c:v>131.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>140</c:v>
+                  <c:v>130.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>139.5</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>139</c:v>
+                  <c:v>129.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>138.5</c:v>
+                  <c:v>128.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>138</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>137.5</c:v>
+                  <c:v>127.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>137</c:v>
+                  <c:v>126.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>136.5</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>136</c:v>
+                  <c:v>125.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>135.5</c:v>
+                  <c:v>124.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>135</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>134.5</c:v>
+                  <c:v>123.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>134</c:v>
+                  <c:v>122.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>133.5</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>133</c:v>
+                  <c:v>121.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>132.5</c:v>
+                  <c:v>120.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>132</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>131.5</c:v>
+                  <c:v>119.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>131</c:v>
+                  <c:v>118.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>130.5</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>130</c:v>
+                  <c:v>117.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>129.5</c:v>
+                  <c:v>116.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>129</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>128.5</c:v>
+                  <c:v>115.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>128</c:v>
+                  <c:v>114.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>127.5</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>127</c:v>
+                  <c:v>113.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>126.5</c:v>
+                  <c:v>112.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>126</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>125.5</c:v>
+                  <c:v>111.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>125</c:v>
+                  <c:v>110.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>124.5</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>124</c:v>
+                  <c:v>109.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>123.5</c:v>
+                  <c:v>108.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>123</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>122.5</c:v>
+                  <c:v>107.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>122</c:v>
+                  <c:v>106.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>121.5</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>121</c:v>
+                  <c:v>105.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>120.5</c:v>
+                  <c:v>104.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>120</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>119.5</c:v>
+                  <c:v>103.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>119</c:v>
+                  <c:v>102.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>118.5</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>118</c:v>
+                  <c:v>101.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>117.5</c:v>
+                  <c:v>100.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>117</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>116.5</c:v>
+                  <c:v>99.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>116</c:v>
+                  <c:v>98.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>115.5</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>115</c:v>
+                  <c:v>97.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>114.5</c:v>
+                  <c:v>96.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>114</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>113.5</c:v>
+                  <c:v>95.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>113</c:v>
+                  <c:v>94.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>112.5</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>112</c:v>
+                  <c:v>93.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>111.5</c:v>
+                  <c:v>92.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>111</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>110.5</c:v>
+                  <c:v>91.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>110</c:v>
+                  <c:v>90.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>109.5</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>109</c:v>
+                  <c:v>89.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>108.5</c:v>
+                  <c:v>88.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>108</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>107.5</c:v>
+                  <c:v>87.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>107</c:v>
+                  <c:v>86.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>106.5</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>106</c:v>
+                  <c:v>85.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>105.5</c:v>
+                  <c:v>84.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>105</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>104.5</c:v>
+                  <c:v>83.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>104</c:v>
+                  <c:v>82.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>103.5</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>103</c:v>
+                  <c:v>81.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>102.5</c:v>
+                  <c:v>80.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>102</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>101.5</c:v>
+                  <c:v>79.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>101</c:v>
+                  <c:v>78.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>100.5</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>100</c:v>
+                  <c:v>77.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>99.5</c:v>
+                  <c:v>76.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>99</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>98.5</c:v>
+                  <c:v>75.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>98</c:v>
+                  <c:v>74.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>97.5</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>97</c:v>
+                  <c:v>73.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>96.5</c:v>
+                  <c:v>72.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>96</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>95.5</c:v>
+                  <c:v>71.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>95</c:v>
+                  <c:v>70.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>94.5</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>94</c:v>
+                  <c:v>69.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>93.5</c:v>
+                  <c:v>68.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>93</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>92.5</c:v>
+                  <c:v>67.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>92</c:v>
+                  <c:v>66.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>91.5</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>91</c:v>
+                  <c:v>65.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>90.5</c:v>
+                  <c:v>64.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>90</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>89.5</c:v>
+                  <c:v>63.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>89</c:v>
+                  <c:v>62.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>88.5</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>88</c:v>
+                  <c:v>61.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>87.5</c:v>
+                  <c:v>60.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>87</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>86.5</c:v>
+                  <c:v>59.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>86</c:v>
+                  <c:v>58.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>85.5</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>85</c:v>
+                  <c:v>57.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>84.5</c:v>
+                  <c:v>56.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>55.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>54.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>53.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>52.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>51.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>50.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>49.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>48.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>47.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>46.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>45.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>43.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>42.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>41.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>40.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>39.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>38.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>37.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>36.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>35.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>34.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>33.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>32.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>31.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>30.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>29.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>28.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>27.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>26.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>25.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>24.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>23.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>22.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>21.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>20.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>19.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>18.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>17.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>16.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>15.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>14.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>13.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>12.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>11.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>10.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>9.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>8.6666666666666572</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>7.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>6.6666666666666572</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>5.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>4.6666666666666572</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>3.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>2.6666666666666572</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1.3333333333333428</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.66666666666665719</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2721,13 +2748,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>304799</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
@@ -3050,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,11 +3126,11 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <f>H2-H3</f>
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3113,12 +3140,12 @@
         <v>168</v>
       </c>
       <c r="I2">
-        <f>(G4-G2)/(I6-H2)</f>
-        <v>-1.1904761904761904E-2</v>
+        <f>(G5-G2)/(H5-H2)</f>
+        <v>-1.7857142857142856E-2</v>
       </c>
       <c r="J2">
         <f>1-(H2*I2)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3127,7 +3154,7 @@
       </c>
       <c r="B3">
         <f>B2-E2</f>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3137,20 +3164,20 @@
       </c>
       <c r="F3">
         <f>H3-H4</f>
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
         <f>(G3-J2)/I2</f>
-        <v>84</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>B3-E3</f>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -3160,14 +3187,14 @@
       </c>
       <c r="F4">
         <f>H4-H5</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <f>(G4-$J$2)/$I$2</f>
-        <v>0</v>
+        <f>(G4-J2)/I2</f>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3175,6 +3202,23 @@
         <v>11</v>
       </c>
       <c r="B5">
+        <f>B4-E4</f>
+        <v>166</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>H5-H6</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
     </row>
@@ -3184,10 +3228,18 @@
       </c>
       <c r="E8">
         <f>COUNT(Sheet2!A:A)</f>
-        <v>337</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3195,10 +3247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B337"/>
+  <dimension ref="A1:B253"/>
   <sheetViews>
-    <sheetView topLeftCell="A300" workbookViewId="0">
-      <selection sqref="A1:B337"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,7 +3271,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>167.5</v>
+        <v>167.33333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3227,7 +3279,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>167</v>
+        <v>166.66666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3235,7 +3287,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>166.5</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3243,7 +3295,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>166</v>
+        <v>165.33333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3251,7 +3303,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>165.5</v>
+        <v>164.66666666666666</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3259,7 +3311,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3267,7 +3319,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>164.5</v>
+        <v>163.33333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3275,7 +3327,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>164</v>
+        <v>162.66666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3283,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>163.5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3291,7 +3343,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>163</v>
+        <v>161.33333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3299,7 +3351,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>162.5</v>
+        <v>160.66666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3307,7 +3359,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3315,7 +3367,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>161.5</v>
+        <v>159.33333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3323,7 +3375,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>161</v>
+        <v>158.66666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3331,7 +3383,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>160.5</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3339,7 +3391,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>160</v>
+        <v>157.33333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,7 +3399,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>159.5</v>
+        <v>156.66666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3355,7 +3407,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3363,7 +3415,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>158.5</v>
+        <v>155.33333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3371,7 +3423,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>158</v>
+        <v>154.66666666666666</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3379,7 +3431,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>157.5</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3387,7 +3439,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>157</v>
+        <v>153.33333333333331</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3395,7 +3447,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>156.5</v>
+        <v>152.66666666666666</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3403,7 +3455,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3411,7 +3463,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>155.5</v>
+        <v>151.33333333333331</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3419,7 +3471,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>155</v>
+        <v>150.66666666666666</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3427,7 +3479,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>154.5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3435,7 +3487,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>154</v>
+        <v>149.33333333333331</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3443,7 +3495,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>153.5</v>
+        <v>148.66666666666666</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3451,7 +3503,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3459,7 +3511,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>152.5</v>
+        <v>147.33333333333331</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3467,7 +3519,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>152</v>
+        <v>146.66666666666666</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3475,7 +3527,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>151.5</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3483,7 +3535,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>151</v>
+        <v>145.33333333333331</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3491,7 +3543,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>150.5</v>
+        <v>144.66666666666666</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3499,7 +3551,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3507,7 +3559,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>149.5</v>
+        <v>143.33333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3515,7 +3567,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>149</v>
+        <v>142.66666666666666</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3523,7 +3575,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>148.5</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3531,7 +3583,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>148</v>
+        <v>141.33333333333331</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3539,7 +3591,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>147.5</v>
+        <v>140.66666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3547,7 +3599,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3555,7 +3607,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>146.5</v>
+        <v>139.33333333333331</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3563,7 +3615,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>146</v>
+        <v>138.66666666666666</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3571,7 +3623,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>145.5</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3579,7 +3631,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>145</v>
+        <v>137.33333333333331</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3587,7 +3639,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>144.5</v>
+        <v>136.66666666666666</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3595,7 +3647,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3603,7 +3655,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>143.5</v>
+        <v>135.33333333333331</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3611,7 +3663,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>143</v>
+        <v>134.66666666666666</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3619,7 +3671,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>142.5</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3627,7 +3679,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>142</v>
+        <v>133.33333333333331</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3635,7 +3687,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>141.5</v>
+        <v>132.66666666666666</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3643,7 +3695,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3651,7 +3703,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>140.5</v>
+        <v>131.33333333333331</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3659,7 +3711,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>140</v>
+        <v>130.66666666666666</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3667,7 +3719,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>139.5</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3675,7 +3727,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>139</v>
+        <v>129.33333333333331</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3683,7 +3735,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>138.5</v>
+        <v>128.66666666666666</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3691,7 +3743,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3699,7 +3751,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>137.5</v>
+        <v>127.33333333333333</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3707,7 +3759,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>137</v>
+        <v>126.66666666666666</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3715,7 +3767,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>136.5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3723,7 +3775,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>136</v>
+        <v>125.33333333333333</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3731,7 +3783,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>135.5</v>
+        <v>124.66666666666666</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3739,7 +3791,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3747,7 +3799,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>134.5</v>
+        <v>123.33333333333333</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3755,7 +3807,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>134</v>
+        <v>122.66666666666666</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3763,7 +3815,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>133.5</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -3771,7 +3823,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>133</v>
+        <v>121.33333333333333</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -3779,7 +3831,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>132.5</v>
+        <v>120.66666666666666</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -3787,7 +3839,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -3795,7 +3847,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>131.5</v>
+        <v>119.33333333333333</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -3803,7 +3855,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>131</v>
+        <v>118.66666666666666</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3811,7 +3863,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>130.5</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3819,7 +3871,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>130</v>
+        <v>117.33333333333333</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -3827,7 +3879,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>129.5</v>
+        <v>116.66666666666666</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -3835,7 +3887,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -3843,7 +3895,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>128.5</v>
+        <v>115.33333333333333</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3851,7 +3903,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>128</v>
+        <v>114.66666666666666</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3859,7 +3911,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>127.5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -3867,7 +3919,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>127</v>
+        <v>113.33333333333333</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -3875,7 +3927,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>126.5</v>
+        <v>112.66666666666666</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3883,7 +3935,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -3891,7 +3943,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>125.5</v>
+        <v>111.33333333333333</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -3899,7 +3951,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>125</v>
+        <v>110.66666666666666</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -3907,7 +3959,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>124.5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -3915,7 +3967,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>124</v>
+        <v>109.33333333333333</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -3923,7 +3975,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>123.5</v>
+        <v>108.66666666666666</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3931,7 +3983,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -3939,7 +3991,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>122.5</v>
+        <v>107.33333333333333</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3947,7 +3999,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>122</v>
+        <v>106.66666666666666</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -3955,7 +4007,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>121.5</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -3963,7 +4015,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>121</v>
+        <v>105.33333333333333</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -3971,7 +4023,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>120.5</v>
+        <v>104.66666666666666</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -3979,7 +4031,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -3987,7 +4039,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>119.5</v>
+        <v>103.33333333333333</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -3995,7 +4047,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>119</v>
+        <v>102.66666666666666</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -4003,7 +4055,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>118.5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -4011,7 +4063,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>118</v>
+        <v>101.33333333333333</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -4019,7 +4071,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>117.5</v>
+        <v>100.66666666666666</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -4027,7 +4079,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -4035,7 +4087,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>116.5</v>
+        <v>99.333333333333329</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -4043,7 +4095,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>116</v>
+        <v>98.666666666666657</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -4051,7 +4103,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>115.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -4059,7 +4111,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>115</v>
+        <v>97.333333333333329</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -4067,7 +4119,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>114.5</v>
+        <v>96.666666666666657</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -4075,7 +4127,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -4083,7 +4135,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>113.5</v>
+        <v>95.333333333333329</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -4091,7 +4143,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>113</v>
+        <v>94.666666666666657</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -4099,7 +4151,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>112.5</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -4107,7 +4159,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>112</v>
+        <v>93.333333333333329</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -4115,7 +4167,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>111.5</v>
+        <v>92.666666666666657</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4123,7 +4175,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -4131,7 +4183,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>110.5</v>
+        <v>91.333333333333329</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -4139,7 +4191,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>110</v>
+        <v>90.666666666666657</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -4147,7 +4199,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>109.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -4155,7 +4207,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>109</v>
+        <v>89.333333333333329</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -4163,7 +4215,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>108.5</v>
+        <v>88.666666666666657</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -4171,7 +4223,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -4179,7 +4231,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>107.5</v>
+        <v>87.333333333333329</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -4187,7 +4239,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>107</v>
+        <v>86.666666666666657</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -4195,7 +4247,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>106.5</v>
+        <v>86</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -4203,7 +4255,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>106</v>
+        <v>85.333333333333329</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -4211,7 +4263,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>105.5</v>
+        <v>84.666666666666657</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -4219,7 +4271,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -4227,7 +4279,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>104.5</v>
+        <v>83.333333333333329</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -4235,7 +4287,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>104</v>
+        <v>82.666666666666657</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -4243,7 +4295,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>103.5</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -4251,7 +4303,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>103</v>
+        <v>81.333333333333329</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -4259,7 +4311,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>102.5</v>
+        <v>80.666666666666657</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -4267,7 +4319,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -4275,7 +4327,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>101.5</v>
+        <v>79.333333333333329</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -4283,7 +4335,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>101</v>
+        <v>78.666666666666657</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -4291,7 +4343,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>100.5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -4299,7 +4351,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>100</v>
+        <v>77.333333333333329</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -4307,7 +4359,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>99.5</v>
+        <v>76.666666666666657</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -4315,7 +4367,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -4323,7 +4375,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>98.5</v>
+        <v>75.333333333333329</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -4331,7 +4383,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>98</v>
+        <v>74.666666666666657</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -4339,7 +4391,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>97.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -4347,7 +4399,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>97</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -4355,7 +4407,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>96.5</v>
+        <v>72.666666666666657</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -4363,7 +4415,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -4371,7 +4423,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>95.5</v>
+        <v>71.333333333333329</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -4379,7 +4431,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>95</v>
+        <v>70.666666666666657</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -4387,7 +4439,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>94.5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -4395,7 +4447,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>94</v>
+        <v>69.333333333333329</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -4403,7 +4455,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>93.5</v>
+        <v>68.666666666666657</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -4411,7 +4463,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -4419,7 +4471,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>92.5</v>
+        <v>67.333333333333329</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -4427,7 +4479,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>92</v>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -4435,7 +4487,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>91.5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -4443,7 +4495,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>91</v>
+        <v>65.333333333333329</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -4451,7 +4503,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>90.5</v>
+        <v>64.666666666666657</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -4459,7 +4511,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -4467,7 +4519,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>89.5</v>
+        <v>63.333333333333329</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -4475,7 +4527,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>89</v>
+        <v>62.666666666666657</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -4483,7 +4535,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>88.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -4491,7 +4543,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>88</v>
+        <v>61.333333333333329</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -4499,7 +4551,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>87.5</v>
+        <v>60.666666666666657</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -4507,7 +4559,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -4515,7 +4567,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>86.5</v>
+        <v>59.333333333333329</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -4523,7 +4575,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>86</v>
+        <v>58.666666666666657</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -4531,7 +4583,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>85.5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -4539,7 +4591,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>85</v>
+        <v>57.333333333333329</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -4547,7 +4599,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>84.5</v>
+        <v>56.666666666666657</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -4555,7 +4607,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -4563,7 +4615,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>83.5</v>
+        <v>55.333333333333329</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -4571,7 +4623,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>83</v>
+        <v>54.666666666666657</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -4579,7 +4631,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>82.5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -4587,7 +4639,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>82</v>
+        <v>53.333333333333329</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -4595,7 +4647,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>81.5</v>
+        <v>52.666666666666657</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -4603,7 +4655,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -4611,7 +4663,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>80.5</v>
+        <v>51.333333333333329</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -4619,7 +4671,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>80</v>
+        <v>50.666666666666657</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -4627,7 +4679,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>79.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -4635,7 +4687,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>79</v>
+        <v>49.333333333333329</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -4643,7 +4695,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>78.5</v>
+        <v>48.666666666666657</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -4651,7 +4703,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -4659,7 +4711,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>77.5</v>
+        <v>47.333333333333329</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -4667,7 +4719,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>77</v>
+        <v>46.666666666666657</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -4675,7 +4727,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>76.5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -4683,7 +4735,7 @@
         <v>185</v>
       </c>
       <c r="B185">
-        <v>76</v>
+        <v>45.333333333333329</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -4691,7 +4743,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>75.5</v>
+        <v>44.666666666666657</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -4699,7 +4751,7 @@
         <v>187</v>
       </c>
       <c r="B187">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -4707,7 +4759,7 @@
         <v>188</v>
       </c>
       <c r="B188">
-        <v>74.5</v>
+        <v>43.333333333333329</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -4715,7 +4767,7 @@
         <v>189</v>
       </c>
       <c r="B189">
-        <v>74</v>
+        <v>42.666666666666657</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -4723,7 +4775,7 @@
         <v>190</v>
       </c>
       <c r="B190">
-        <v>73.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -4731,7 +4783,7 @@
         <v>191</v>
       </c>
       <c r="B191">
-        <v>73</v>
+        <v>41.333333333333329</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -4739,7 +4791,7 @@
         <v>192</v>
       </c>
       <c r="B192">
-        <v>72.5</v>
+        <v>40.666666666666657</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -4747,7 +4799,7 @@
         <v>193</v>
       </c>
       <c r="B193">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -4755,7 +4807,7 @@
         <v>194</v>
       </c>
       <c r="B194">
-        <v>71.5</v>
+        <v>39.333333333333343</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -4763,7 +4815,7 @@
         <v>195</v>
       </c>
       <c r="B195">
-        <v>71</v>
+        <v>38.666666666666657</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -4771,7 +4823,7 @@
         <v>196</v>
       </c>
       <c r="B196">
-        <v>70.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -4779,7 +4831,7 @@
         <v>197</v>
       </c>
       <c r="B197">
-        <v>70</v>
+        <v>37.333333333333343</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -4787,7 +4839,7 @@
         <v>198</v>
       </c>
       <c r="B198">
-        <v>69.5</v>
+        <v>36.666666666666657</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -4795,7 +4847,7 @@
         <v>199</v>
       </c>
       <c r="B199">
-        <v>69</v>
+        <v>36</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -4803,7 +4855,7 @@
         <v>200</v>
       </c>
       <c r="B200">
-        <v>68.5</v>
+        <v>35.333333333333343</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -4811,7 +4863,7 @@
         <v>201</v>
       </c>
       <c r="B201">
-        <v>68</v>
+        <v>34.666666666666657</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -4819,7 +4871,7 @@
         <v>202</v>
       </c>
       <c r="B202">
-        <v>67.5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -4827,7 +4879,7 @@
         <v>203</v>
       </c>
       <c r="B203">
-        <v>67</v>
+        <v>33.333333333333343</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -4835,7 +4887,7 @@
         <v>204</v>
       </c>
       <c r="B204">
-        <v>66.5</v>
+        <v>32.666666666666657</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -4843,7 +4895,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -4851,7 +4903,7 @@
         <v>206</v>
       </c>
       <c r="B206">
-        <v>65.5</v>
+        <v>31.333333333333343</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -4859,7 +4911,7 @@
         <v>207</v>
       </c>
       <c r="B207">
-        <v>65</v>
+        <v>30.666666666666657</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -4867,7 +4919,7 @@
         <v>208</v>
       </c>
       <c r="B208">
-        <v>64.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -4875,7 +4927,7 @@
         <v>209</v>
       </c>
       <c r="B209">
-        <v>64</v>
+        <v>29.333333333333343</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -4883,7 +4935,7 @@
         <v>210</v>
       </c>
       <c r="B210">
-        <v>63.5</v>
+        <v>28.666666666666657</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -4891,7 +4943,7 @@
         <v>211</v>
       </c>
       <c r="B211">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -4899,7 +4951,7 @@
         <v>212</v>
       </c>
       <c r="B212">
-        <v>62.5</v>
+        <v>27.333333333333343</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -4907,7 +4959,7 @@
         <v>213</v>
       </c>
       <c r="B213">
-        <v>62</v>
+        <v>26.666666666666657</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -4915,7 +4967,7 @@
         <v>214</v>
       </c>
       <c r="B214">
-        <v>61.5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -4923,7 +4975,7 @@
         <v>215</v>
       </c>
       <c r="B215">
-        <v>61</v>
+        <v>25.333333333333343</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -4931,7 +4983,7 @@
         <v>216</v>
       </c>
       <c r="B216">
-        <v>60.5</v>
+        <v>24.666666666666657</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -4939,7 +4991,7 @@
         <v>217</v>
       </c>
       <c r="B217">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -4947,7 +4999,7 @@
         <v>218</v>
       </c>
       <c r="B218">
-        <v>59.5</v>
+        <v>23.333333333333343</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -4955,7 +5007,7 @@
         <v>219</v>
       </c>
       <c r="B219">
-        <v>59</v>
+        <v>22.666666666666657</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -4963,7 +5015,7 @@
         <v>220</v>
       </c>
       <c r="B220">
-        <v>58.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -4971,7 +5023,7 @@
         <v>221</v>
       </c>
       <c r="B221">
-        <v>58</v>
+        <v>21.333333333333343</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -4979,7 +5031,7 @@
         <v>222</v>
       </c>
       <c r="B222">
-        <v>57.5</v>
+        <v>20.666666666666657</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -4987,7 +5039,7 @@
         <v>223</v>
       </c>
       <c r="B223">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -4995,7 +5047,7 @@
         <v>224</v>
       </c>
       <c r="B224">
-        <v>56.5</v>
+        <v>19.333333333333343</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -5003,7 +5055,7 @@
         <v>225</v>
       </c>
       <c r="B225">
-        <v>56</v>
+        <v>18.666666666666657</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -5011,7 +5063,7 @@
         <v>226</v>
       </c>
       <c r="B226">
-        <v>55.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -5019,7 +5071,7 @@
         <v>227</v>
       </c>
       <c r="B227">
-        <v>55</v>
+        <v>17.333333333333343</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -5027,7 +5079,7 @@
         <v>228</v>
       </c>
       <c r="B228">
-        <v>54.5</v>
+        <v>16.666666666666657</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -5035,7 +5087,7 @@
         <v>229</v>
       </c>
       <c r="B229">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -5043,7 +5095,7 @@
         <v>230</v>
       </c>
       <c r="B230">
-        <v>53.5</v>
+        <v>15.333333333333343</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -5051,7 +5103,7 @@
         <v>231</v>
       </c>
       <c r="B231">
-        <v>53</v>
+        <v>14.666666666666657</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -5059,7 +5111,7 @@
         <v>232</v>
       </c>
       <c r="B232">
-        <v>52.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -5067,7 +5119,7 @@
         <v>233</v>
       </c>
       <c r="B233">
-        <v>52</v>
+        <v>13.333333333333343</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -5075,7 +5127,7 @@
         <v>234</v>
       </c>
       <c r="B234">
-        <v>51.5</v>
+        <v>12.666666666666657</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -5083,7 +5135,7 @@
         <v>235</v>
       </c>
       <c r="B235">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -5091,7 +5143,7 @@
         <v>236</v>
       </c>
       <c r="B236">
-        <v>50.5</v>
+        <v>11.333333333333343</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -5099,7 +5151,7 @@
         <v>237</v>
       </c>
       <c r="B237">
-        <v>50</v>
+        <v>10.666666666666657</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -5107,7 +5159,7 @@
         <v>238</v>
       </c>
       <c r="B238">
-        <v>49.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -5115,7 +5167,7 @@
         <v>239</v>
       </c>
       <c r="B239">
-        <v>49</v>
+        <v>9.3333333333333428</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -5123,7 +5175,7 @@
         <v>240</v>
       </c>
       <c r="B240">
-        <v>48.5</v>
+        <v>8.6666666666666572</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -5131,7 +5183,7 @@
         <v>241</v>
       </c>
       <c r="B241">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -5139,7 +5191,7 @@
         <v>242</v>
       </c>
       <c r="B242">
-        <v>47.5</v>
+        <v>7.3333333333333428</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -5147,7 +5199,7 @@
         <v>243</v>
       </c>
       <c r="B243">
-        <v>47</v>
+        <v>6.6666666666666572</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -5155,7 +5207,7 @@
         <v>244</v>
       </c>
       <c r="B244">
-        <v>46.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -5163,7 +5215,7 @@
         <v>245</v>
       </c>
       <c r="B245">
-        <v>46</v>
+        <v>5.3333333333333428</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -5171,7 +5223,7 @@
         <v>246</v>
       </c>
       <c r="B246">
-        <v>45.5</v>
+        <v>4.6666666666666572</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -5179,7 +5231,7 @@
         <v>247</v>
       </c>
       <c r="B247">
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -5187,7 +5239,7 @@
         <v>248</v>
       </c>
       <c r="B248">
-        <v>44.5</v>
+        <v>3.3333333333333428</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -5195,7 +5247,7 @@
         <v>249</v>
       </c>
       <c r="B249">
-        <v>44</v>
+        <v>2.6666666666666572</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -5203,7 +5255,7 @@
         <v>250</v>
       </c>
       <c r="B250">
-        <v>43.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -5211,7 +5263,7 @@
         <v>251</v>
       </c>
       <c r="B251">
-        <v>43</v>
+        <v>1.3333333333333428</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -5219,7 +5271,7 @@
         <v>252</v>
       </c>
       <c r="B252">
-        <v>42.5</v>
+        <v>0.66666666666665719</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -5227,678 +5279,6 @@
         <v>253</v>
       </c>
       <c r="B253">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254">
-        <v>254</v>
-      </c>
-      <c r="B254">
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255">
-        <v>255</v>
-      </c>
-      <c r="B255">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256">
-        <v>256</v>
-      </c>
-      <c r="B256">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257">
-        <v>257</v>
-      </c>
-      <c r="B257">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258">
-        <v>258</v>
-      </c>
-      <c r="B258">
-        <v>39.5</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259">
-        <v>259</v>
-      </c>
-      <c r="B259">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260">
-        <v>260</v>
-      </c>
-      <c r="B260">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261">
-        <v>261</v>
-      </c>
-      <c r="B261">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262">
-        <v>262</v>
-      </c>
-      <c r="B262">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263">
-        <v>263</v>
-      </c>
-      <c r="B263">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264">
-        <v>264</v>
-      </c>
-      <c r="B264">
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265">
-        <v>265</v>
-      </c>
-      <c r="B265">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266">
-        <v>266</v>
-      </c>
-      <c r="B266">
-        <v>35.5</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267">
-        <v>267</v>
-      </c>
-      <c r="B267">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268">
-        <v>268</v>
-      </c>
-      <c r="B268">
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269">
-        <v>269</v>
-      </c>
-      <c r="B269">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270">
-        <v>270</v>
-      </c>
-      <c r="B270">
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271">
-        <v>271</v>
-      </c>
-      <c r="B271">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272">
-        <v>272</v>
-      </c>
-      <c r="B272">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273">
-        <v>273</v>
-      </c>
-      <c r="B273">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274">
-        <v>274</v>
-      </c>
-      <c r="B274">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275">
-        <v>275</v>
-      </c>
-      <c r="B275">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276">
-        <v>276</v>
-      </c>
-      <c r="B276">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277">
-        <v>277</v>
-      </c>
-      <c r="B277">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278">
-        <v>278</v>
-      </c>
-      <c r="B278">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279">
-        <v>279</v>
-      </c>
-      <c r="B279">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280">
-        <v>280</v>
-      </c>
-      <c r="B280">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281">
-        <v>281</v>
-      </c>
-      <c r="B281">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282">
-        <v>282</v>
-      </c>
-      <c r="B282">
-        <v>27.5</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283">
-        <v>283</v>
-      </c>
-      <c r="B283">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284">
-        <v>284</v>
-      </c>
-      <c r="B284">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285">
-        <v>285</v>
-      </c>
-      <c r="B285">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286">
-        <v>286</v>
-      </c>
-      <c r="B286">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287">
-        <v>287</v>
-      </c>
-      <c r="B287">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288">
-        <v>288</v>
-      </c>
-      <c r="B288">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289">
-        <v>289</v>
-      </c>
-      <c r="B289">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290">
-        <v>290</v>
-      </c>
-      <c r="B290">
-        <v>23.5</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291">
-        <v>291</v>
-      </c>
-      <c r="B291">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292">
-        <v>292</v>
-      </c>
-      <c r="B292">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293">
-        <v>293</v>
-      </c>
-      <c r="B293">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294">
-        <v>294</v>
-      </c>
-      <c r="B294">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295">
-        <v>295</v>
-      </c>
-      <c r="B295">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296">
-        <v>296</v>
-      </c>
-      <c r="B296">
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297">
-        <v>297</v>
-      </c>
-      <c r="B297">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298">
-        <v>298</v>
-      </c>
-      <c r="B298">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299">
-        <v>299</v>
-      </c>
-      <c r="B299">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300">
-        <v>300</v>
-      </c>
-      <c r="B300">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301">
-        <v>301</v>
-      </c>
-      <c r="B301">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302">
-        <v>302</v>
-      </c>
-      <c r="B302">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303">
-        <v>303</v>
-      </c>
-      <c r="B303">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304">
-        <v>304</v>
-      </c>
-      <c r="B304">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305">
-        <v>305</v>
-      </c>
-      <c r="B305">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306">
-        <v>306</v>
-      </c>
-      <c r="B306">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307">
-        <v>307</v>
-      </c>
-      <c r="B307">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308">
-        <v>308</v>
-      </c>
-      <c r="B308">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309">
-        <v>309</v>
-      </c>
-      <c r="B309">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310">
-        <v>310</v>
-      </c>
-      <c r="B310">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311">
-        <v>311</v>
-      </c>
-      <c r="B311">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312">
-        <v>312</v>
-      </c>
-      <c r="B312">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313">
-        <v>313</v>
-      </c>
-      <c r="B313">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314">
-        <v>314</v>
-      </c>
-      <c r="B314">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315">
-        <v>315</v>
-      </c>
-      <c r="B315">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316">
-        <v>316</v>
-      </c>
-      <c r="B316">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317">
-        <v>317</v>
-      </c>
-      <c r="B317">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318">
-        <v>318</v>
-      </c>
-      <c r="B318">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319">
-        <v>319</v>
-      </c>
-      <c r="B319">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320">
-        <v>320</v>
-      </c>
-      <c r="B320">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321">
-        <v>321</v>
-      </c>
-      <c r="B321">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322">
-        <v>322</v>
-      </c>
-      <c r="B322">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323">
-        <v>323</v>
-      </c>
-      <c r="B323">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324">
-        <v>324</v>
-      </c>
-      <c r="B324">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325">
-        <v>325</v>
-      </c>
-      <c r="B325">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326">
-        <v>326</v>
-      </c>
-      <c r="B326">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327">
-        <v>327</v>
-      </c>
-      <c r="B327">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328">
-        <v>328</v>
-      </c>
-      <c r="B328">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329">
-        <v>329</v>
-      </c>
-      <c r="B329">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330">
-        <v>330</v>
-      </c>
-      <c r="B330">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331">
-        <v>331</v>
-      </c>
-      <c r="B331">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332">
-        <v>332</v>
-      </c>
-      <c r="B332">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333">
-        <v>333</v>
-      </c>
-      <c r="B333">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334">
-        <v>334</v>
-      </c>
-      <c r="B334">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335">
-        <v>335</v>
-      </c>
-      <c r="B335">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336">
-        <v>336</v>
-      </c>
-      <c r="B336">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337">
-        <v>337</v>
-      </c>
-      <c r="B337">
         <v>0</v>
       </c>
     </row>

</xml_diff>